<commit_message>
CPI corrected, new Plots
</commit_message>
<xml_diff>
--- a/data/processed/climate_df.xlsx
+++ b/data/processed/climate_df.xlsx
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>134.9580258844471</v>
+        <v>491.9042826293455</v>
       </c>
       <c r="D2" t="n">
         <v>2.455315637441395</v>
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37.94784849573697</v>
+        <v>138.3149247278208</v>
       </c>
       <c r="D3" t="n">
         <v>0.2068543207077463</v>
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7.078988154845171</v>
+        <v>25.80198226248687</v>
       </c>
       <c r="D4" t="n">
         <v>0.4871875536948298</v>
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15.41767263196158</v>
+        <v>56.19539220537131</v>
       </c>
       <c r="D5" t="n">
         <v>0.3910269294331641</v>
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-8.988842561602185</v>
+        <v>-32.76315078674113</v>
       </c>
       <c r="D6" t="n">
         <v>0.639111105717419</v>

</xml_diff>

<commit_message>
New country level SLAND values GCB2023
</commit_message>
<xml_diff>
--- a/data/processed/climate_df.xlsx
+++ b/data/processed/climate_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,65 +456,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>SLAND_corrected</t>
+          <t>ELUC</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>SLAND_dor</t>
+          <t>EFOS</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ELUC</t>
+          <t>F_ab</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>EFOS</t>
+          <t>F_ac</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>F_ab</t>
+          <t>F_abc</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>F_ac</t>
+          <t>continent</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>F_abc</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>F_ab_cor</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>F_abc_cor</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>F_ab_dor</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>F_abc_dor</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>continent</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>economic_group</t>
         </is>
@@ -528,56 +498,38 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AGOARGATGBDIBENBFABGDBHSBLZBOLBRABRBBRNCAFCIVCMRCODCOGCOKCOLCOMCRICUBDMADOMECUETHFJIFSMGABGHAGINGMBGNBGNQGRDGTMGUYHNDHTIIDNINDJAMKENKHMKIRKNALAOLBRLCALKAMDGMDVMEXMHLMMRMOZMUSMWIMYSNGANICNIUNRUPANPERPHLPLWPNGPRYRWASENSGPSLBSLESLVSTPSURSWZSYCTGOTHATLSTONTTOTUVTZAUGAURYVCTVENVNMVUTWSMZMB</t>
+          <t>AGOARGBDIBENBFABGDBHSBLZBOLBRABRNCAFCIVCMRCODCOGCOKCOLCOMCRICUBDOMECUETHFJIGABGHAGINGMBGNBGNQGTMGUYHNDHTIIDNINDJAMKENKHMKIRLAOLBRLKAMDGMEXMMRMOZMUSMWIMYSNGANICPANPERPHLPNGPRYRWASENSLBSLESLVSTPSURSWZTGOTHATLSTTOTZAUGAURYVCTVENVNMVUTWSMZMB</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>491.9042826293455</v>
+        <v>479.5156661484671</v>
       </c>
       <c r="D2" t="n">
-        <v>2.455315637441395</v>
+        <v>1.831527709960938</v>
       </c>
       <c r="E2" t="n">
-        <v>1.865482965280907</v>
+        <v>-1.11149014075</v>
       </c>
       <c r="F2" t="n">
-        <v>1.559344984318135</v>
+        <v>-1.641572104287398</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.070532937499999</v>
+        <v>0.7200375850197459</v>
       </c>
       <c r="H2" t="n">
-        <v>-1.70424158035719</v>
+        <v>-2.753062245037398</v>
       </c>
       <c r="I2" t="n">
-        <v>1.384782699941394</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-2.77477451785719</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-0.3194588804158007</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.794950027780908</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-0.9092915525762835</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.4888120468181337</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-1.215429533539058</v>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>AfricaLatin America and the CaribbeanLatin America and the CaribbeanAfricaAfricaAfricaAsiaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAsiaAfricaAfricaAfricaAfricaAfricaOceaniaLatin America and the CaribbeanAfricaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAfricaOceaniaOceaniaAfricaAfricaAfricaAfricaAfricaAfricaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAsiaAsiaLatin America and the CaribbeanAfricaAsiaOceaniaLatin America and the CaribbeanAsiaAfricaLatin America and the CaribbeanAsiaAfricaAsiaLatin America and the CaribbeanOceaniaAsiaAfricaAfricaAfricaAsiaAfricaLatin America and the CaribbeanOceaniaOceaniaLatin America and the CaribbeanLatin America and the CaribbeanAsiaOceaniaOceaniaLatin America and the CaribbeanAfricaAfricaAsiaOceaniaAfricaLatin America and the CaribbeanAfricaLatin America and the CaribbeanAfricaAfricaAfricaAsiaAsiaOceaniaLatin America and the CaribbeanOceaniaAfricaAfricaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAsiaOceaniaOceaniaAfrica</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>LDCOtherOtherLDCLDCLDCOtherOtherOtherOtherBRICSOtherOtherLDCOtherOtherLDCOtherOtherOECDLDCOECDOtherOtherOtherOtherBRICSOtherOtherOtherOtherLDCLDCLDCOtherOtherOtherOtherOtherLDCOtherBRICSOtherOtherLDCOtherOtherLDCLDCOtherOtherLDCOtherOECDOtherLDCLDCOtherLDCOtherOtherOtherOtherOtherOtherOtherOtherOtherOtherOtherLDCLDCOtherOtherLDCOtherLDCOtherLDCOtherLDCOtherLDCOtherOtherOtherLDCLDCOtherOtherOtherOtherOtherOtherLDC</t>
+        <v>-0.9215345192676525</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>AfricaLatin America and the CaribbeanAfricaAfricaAfricaAsiaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAsiaAfricaAfricaAfricaAfricaAfricaOceaniaLatin America and the CaribbeanAfricaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAfricaOceaniaAfricaAfricaAfricaAfricaAfricaAfricaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAsiaAsiaLatin America and the CaribbeanAfricaAsiaOceaniaAsiaAfricaAsiaAfricaLatin America and the CaribbeanAsiaAfricaAfricaAfricaAsiaAfricaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAsiaOceaniaLatin America and the CaribbeanAfricaAfricaOceaniaAfricaLatin America and the CaribbeanAfricaLatin America and the CaribbeanAfricaAfricaAsiaAsiaLatin America and the CaribbeanAfricaAfricaLatin America and the CaribbeanLatin America and the CaribbeanLatin America and the CaribbeanAsiaOceaniaOceaniaAfrica</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>LDCOtherLDCLDCLDCOtherOtherOtherOtherBRICSOtherLDCOtherOtherLDCOtherOtherOECDLDCOECDOtherOtherOtherBRICSOtherOtherOtherLDCLDCLDCOtherOtherOtherOtherLDCOtherBRICSOtherOtherLDCOtherLDCLDCOtherLDCOECDLDCLDCOtherLDCOtherOtherOtherOtherOtherOtherOtherOtherLDCLDCOtherLDCOtherLDCOtherLDCLDCOtherLDCOtherLDCLDCOtherOtherOtherOtherOtherOtherLDC</t>
         </is>
       </c>
     </row>
@@ -589,56 +541,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AREAUSBHRBWACHLCPVDJIDZAEGYERIIRNIRQISRJORKWTLBYLSOMARMLIMRTNAMNEROMNPAKPSEQATSAUSDNSOMSSDSYRTCDTKMTUNYEMZAFZWE</t>
+          <t>AREAUSBWACHLCPVDJIDZAEGYERIIRNIRQISRJORKWTLBYLSOMARMLIMRTNAMNEROMNPAKPSEQATSAUSDNSOMSOMSSDSYRTCDTKMTUNYEMZAFZWE</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>138.3149247278208</v>
+        <v>134.9298307888636</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2068543207077463</v>
+        <v>0.1445359289646149</v>
       </c>
       <c r="E3" t="n">
-        <v>0.157162364663294</v>
+        <v>-0.05673168899999999</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2068459777754842</v>
+        <v>-1.040377085387413</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0508238942499995</v>
+        <v>0.0878042482414714</v>
       </c>
       <c r="H3" t="n">
-        <v>-1.062960502909167</v>
+        <v>-1.097108774387412</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1560304264577461</v>
-      </c>
-      <c r="J3" t="n">
-        <v>-1.113784397159167</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-0.9069300764514215</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.1063384704132945</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-0.9566220324958723</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.1560220835254844</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-0.9069384193836834</v>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>AsiaOceaniaAsiaAfricaLatin America and the CaribbeanAfricaAfricaAfricaAfricaAfricaAsiaAsiaAsiaAsiaAsiaAfricaAfricaAfricaAfricaAfricaAfricaAfricaAsiaAsiaAsiaAsiaAsiaAfricaAfricaAfricaAsiaAfricaAsiaAfricaAsiaAfricaAfrica</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>BRICSOECDOtherOtherOECDOtherLDCOtherBRICSLDCBRICSOtherOECDOtherOtherOtherLDCOtherLDCOtherOtherLDCOtherOtherOtherOtherOtherOtherOtherLDCOtherLDCOtherOtherOtherBRICSLDC</t>
+        <v>-0.9525728371459411</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>AsiaOceaniaAfricaLatin America and the CaribbeanAfricaAfricaAfricaAfricaAfricaAsiaAsiaAsiaAsiaAsiaAfricaAfricaAfricaAfricaAfricaAfricaAfricaAsiaAsiaAsiaAsiaAsiaAfricaAfricaAfricaAfricaAsiaAfricaAsiaAfricaAsiaAfricaAfrica</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>BRICSOECDOtherOECDOtherLDCOtherBRICSLDCBRICSOtherOECDOtherOtherOtherLDCOtherLDCOtherOtherLDCOtherOtherOtherOtherOtherOtherOtherOtherLDCOtherLDCOtherOtherOtherBRICSLDC</t>
         </is>
       </c>
     </row>
@@ -650,56 +584,38 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ALBANDAUTBELBGRBIHCHECYPCZEDEUDNKESPFRAGBRGRCHRVHUNIRLITAJPNKORLBNLIELUXMKDMLTMNENLDNZLPRTROUSRBSVKSVNUSA</t>
+          <t>ALBAUTBELBGRBIHCHECYPCZEDEUDNKESPFRAGBRGRCHRVHUNIRLITAJPNKORLBNLUXMKDMNENLDNZLPRTROUSRBSVKSVNUSA</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>25.80198226248687</v>
+        <v>25.15215896558901</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4871875536948298</v>
+        <v>0.3941102623939514</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3701520360378812</v>
+        <v>0.04610860625</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3140530637630035</v>
+        <v>-2.757478497830251</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0405862089999993</v>
+        <v>0.4402188742900945</v>
       </c>
       <c r="H4" t="n">
-        <v>-2.710730326547989</v>
+        <v>-2.711369891580251</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5277737626948295</v>
-      </c>
-      <c r="J4" t="n">
-        <v>-2.670144117547989</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-2.182956563853159</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.4107382450378815</v>
-      </c>
-      <c r="M4" t="n">
-        <v>-2.299992081510106</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.3546392727630023</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-2.356091053784986</v>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>EuropeEuropeEuropeEuropeEuropeEuropeEuropeAsiaEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeAsiaAsiaAsiaEuropeEuropeEuropeEuropeEuropeEuropeOceaniaEuropeEuropeEuropeEuropeEuropeNorth America</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>OtherOtherOECDOECDOtherOtherOECDOtherOECDOECDOECDOECDOECDOECDOECDOtherOECDOECDOECDOECDOECDOtherOtherOECDOtherOtherOtherOECDOECDOECDOtherOtherOECDOECDOECD</t>
+        <v>-2.317259623540156</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>EuropeEuropeEuropeEuropeEuropeEuropeAsiaEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeEuropeAsiaAsiaAsiaEuropeEuropeEuropeEuropeOceaniaEuropeEuropeEuropeEuropeEuropeNorth America</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>OtherOECDOECDOtherOtherOECDOtherOECDOECDOECDOECDOECDOECDOECDOtherOECDOECDOECDOECDOECDOtherOECDOtherOtherOECDOECDOECDOtherOtherOECDOECDOECD</t>
         </is>
       </c>
     </row>
@@ -715,50 +631,32 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>56.19539220537131</v>
+        <v>54.78011043896012</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3910269294331641</v>
+        <v>0.3781403601169586</v>
       </c>
       <c r="E5" t="n">
-        <v>0.297091772927332</v>
+        <v>0.03537037825</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3278031172037572</v>
+        <v>-3.310600968240123</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0390905295000001</v>
+        <v>0.4135107224908191</v>
       </c>
       <c r="H5" t="n">
-        <v>-3.362956376886574</v>
+        <v>-3.275230589990122</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4301174589331638</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-3.323865847386574</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-2.93283891795341</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.336182302427332</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-3.026774074459242</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.3668936467037569</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-2.996062730182817</v>
-      </c>
-      <c r="P5" t="inlineStr">
+        <v>-2.897090245749303</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>AsiaAsiaAsiaEuropeAsiaAsiaEuropeEuropeAsiaAsiaAsiaEuropeEuropeEuropeAsiaAsiaEuropeAsiaEuropeAsiaAsiaEuropeAsia</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>LDCOtherOtherOtherOtherBRICSOECDOECDOtherOtherOtherOECDOECDOtherOtherOtherOECDOtherOECDOtherOECDOtherOther</t>
         </is>
@@ -776,50 +674,32 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-32.76315078674113</v>
+        <v>-31.93801035976101</v>
       </c>
       <c r="D6" t="n">
-        <v>0.639111105717419</v>
+        <v>0.6215693950653076</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4855794759976759</v>
+        <v>-0.0877665435</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5800490009582129</v>
+        <v>-0.6239657808630126</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.08936996375</v>
+        <v>0.5338028868391501</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.6280754358424481</v>
+        <v>-0.7117323243630125</v>
       </c>
       <c r="I6" t="n">
-        <v>0.549741141967419</v>
-      </c>
-      <c r="J6" t="n">
-        <v>-0.7174453995924481</v>
-      </c>
-      <c r="K6" t="n">
-        <v>-0.0783342938750293</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.3962095122476759</v>
-      </c>
-      <c r="M6" t="n">
-        <v>-0.2318659235947721</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.4906790372082129</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-0.1373963986342353</v>
-      </c>
-      <c r="P6" t="inlineStr">
+        <v>-0.09016289402386246</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>North AmericaEuropeEuropeAsia</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>OECDOECDOECDBRICS</t>
         </is>

</xml_diff>